<commit_message>
Zoomtv Status Code in Excel
</commit_message>
<xml_diff>
--- a/LinkStatus.xlsx
+++ b/LinkStatus.xlsx
@@ -8,24 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RABINDRA SRIVASTAVA\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F155FA-696C-41E6-8D5B-9DCC99039B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E17B020-F1CC-4EE8-928C-52FCF9AE1700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LinkStatus" sheetId="1" r:id="rId1"/>
+    <sheet name="ZoomLinkStatus" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="240">
   <si>
     <t>Status Code</t>
   </si>
@@ -292,13 +288,466 @@
   </si>
   <si>
     <t>https://www.izooto.com/campaign/getting-started-with-web-push-notifications-izooto?utm_source=referral&amp;utm_medium=PoweredBy&amp;utm_campaign=https%3A%2F%2Ftelugu.timesnownews.com</t>
+  </si>
+  <si>
+    <t>URLs</t>
+  </si>
+  <si>
+    <t>https://www.timesnownews.com/</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/hindi</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/#</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/latest-news</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/celebrity</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/bollywood</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/photos</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/videos</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/hollywood</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/telly-talk</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-series</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/korean</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/live-tv</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/photos/celebs</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/videos/bollywood-news-gossips</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/videos/tv-news</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/videos/tv-shows</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/videos/tv-serial-updates</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/videos/specials</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/videos/web-series</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/videos/bollywood-movie-reviews</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/entertainment</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/lifestyle</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/astrology</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/celebrity</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/fashion</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/beauty</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/health</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/travel</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/movies</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/short-videos</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/viral</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/reviews</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/tamil-cinema</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/telugu-cinema</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/malayalam-cinema</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/kannada-cinema</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/travel</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/beauty</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/grooming</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/health-fitness</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/fashion</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/relationships</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/best-of</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-series/exclusive-maanvi-gagroo-on-having-good-and-bad-days-for-public-appearances-learnt-to-live-with-them-article-105187021</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/entertainment/top-10-movies-to-watch-on-ott-on-bhai-dooj-2023-netflix-amazon-prime-video-disney-hotstar-zee5-sony-liv/photostory/105191581.cms</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/korean/bts-jungkooks-debut-days-a-cringeworthy-comedy-of-errors-article-105188325</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/celebrity/salman-khan-and-shah-rukh-khan-spotted-in-deep-conversation-at-arpita-khans-diwali-bash-what-were-they-discussing-article-105190078</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/celebrity/what-mrunal-thakur-spotted-holding-badshahs-hand-at-shilpa-shettys-diwali-party-article-105191378</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/celebrity/exclusive-arjun-kapoor-watches-tiger-3-in-cinemas-puts-cold-war-with-salman-khan-to-an-end-article-105190631</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/short-videos/amitabh-bachchan-reacts-to-fans-strict-warning-over-not-attending-world-cup-final-shorts-reels-105283321</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/telly-talk/elvish-yadav-snake-venom-case-prime-accused-rahul-to-be-in-police-remand-for-another-day-tv-news-entertainment-news-article-105286879</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/celebrity/exclusive-the-buckingham-murders-director-hansal-mehta-calls-kareena-kapoor-easy-and-professional-to-work-with-bollywood-news-entertainment-news-article-105285549</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/celebrity/delhi-high-court-schedules-hearing-of-sushant-singh-rajputs-fathers-plea-against-film-nyay-the-justice-in-2024-bollywood-news-entertainment-news-article-105284294</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/bollywood/tiger-3-box-office-collection-day-5-salman-khan-katrina-kaif-starrer-records-further-dip-bollywood-news-entertainment-news-article-105285062</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/celebrity/parineeti-chopra-approved-ethnic-fits-for-wedding-season/photostory/105286393.cms</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-series/prince-harry-to-skip-the-crown-season-season-6-find-out-why-article-105285146</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/telugu-cinema/karthikeya-2-star-nikhil-siddhartha-wife-dr-pallavi-varma-all-set-to-welcome-first-child-entertainment-news-article-105283799</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/tamil-cinema/rajinikanth-praises-jigarthanda-doublex-ranbir-kapoor-to-appear-on-nandamuri-balakrishnas-talk-show-beyond-bollywood-entertainment-news-article-105283564</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/travel/heres-why-meghalaya-is-the-perfect-winter-destination-article-105252816</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/celebrity/frame-worthy-clicks-of-aaradhya-with-parents-aishwarya-rai-bachchan-abhishek-bachchan/photostory/105284107.cms</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/reviews/khichdi-2-movie-review-parekh-family-takes-us-on-crazy-adventure-review-105277827</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/reviews/phoenix-movie-review-compelling-tale-of-love-and-horror-ft-aju-varghese-anoop-menon-review-105270728</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/telly-talk/tv-wrap-anupama-to-lose-choti-anu-in-anupamaa-manish-and-akshu-come-face-to-face-in-yeh-rishta-kya-kehlata-hai-article-105273856</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/telly-talk/reality-tv-check-ankita-lokhande-undergoes-pregnancy-test-in-bigg-boss-17-nikita-bhamidipati-calls-chetna-pande-gold-digger-article-105271596</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/reviews/spark-life-review-vikranth-reddy-mehreen-pirzadas-film-is-a-hot-mess-review-105269495</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/reviews/trolls-band-together-movie-review-justin-timberlake-unleashes-barrage-of-nostalgic-puns-and-jokes-review-105234291</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/reviews/sesham-mikeil-fathima-movie-review-kalyani-priyadarshans-film-is-about-malabari-muslim-woman-aspiring-to-be-football-commentator-review-105277747</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/reviews/rustin-movie-review-a-biographical-flaw-or-insightful-commentary-on-american-history-review-105269803</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/reviews/sapta-sagaradaache-ello-side-b-movie-review-rakshit-shetty-starrer-gets-darker-review-105276474</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/reviews/anveshi-movie-review-vijay-dharans-film-unveils-mysteries-in-a-riveting-tale-of-love-horror-and-suspense-review-105267166</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/reviews/mangalavaaram-movie-review-ajay-bhupathi-film-sees-payal-rajput-in-an-intriguing-role-review-105270197</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/celebrity/alia-bhatt-breaks-silence-on-ranbir-kapoor-being-labelled-as-toxic-on-kwk-this-is-getting-a-little-out-of-hand-article-105268969</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/celebrity/koffee-with-karan-8-kareena-kapoor-feels-hubby-saif-ali-khan-was-busy-building-his-career-during-sara-ali-kahan-ibrahim-ali-khans-childhood-article-105269032</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/celebrity/kareena-kapoors-kgf-obsession-actress-expresses-desire-to-work-with-yash-article-105265836</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/korean/bts-star-vs-concerning-weverse-message-has-army-sending-him-well-wishes-know-why-article-105266468</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/photos/celebs/international/emily-ratajkowski-sculpted-beauty-photo-gallery-105242414</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/photos/celebs/international/irina-shayk-a-true-bikini-icon-photo-gallery-105215030</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/photos/celebs/bollywood/celebrating-half-decade-of-deep-veer-unbroken-love-photo-gallery-105205879</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/photos/celebs/international/khloe-kardashian-jaw-dropping-moments-unleashed-photo-gallery-105183267</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/bollywood/exclusive-tiger-3-witnesses-50-dip-trade-expert-says-salman-khan-film-doesnt-have-staying-power-bollywood-news-entertainment-news-article-105266701</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/bollywood/todays-ent-wrap-zoya-reveals-she-wasnt-sure-to-cast-star-kids-in-the-archies-is-priyanka-joining-don-3-article-105262233</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/bollywood/katrina-kaif-vijay-sethupathis-merry-christmas-gets-postponed-to-release-on-january-2024-bollywood-news-entertainment-news-article-105255332</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/bollywood/tiger-3-box-office-collection-day-4-salman-khan-starrer-sees-a-dip-earns-rs-169-5-crore-in-india-bollywood-news-entertainment-news-article-105254435</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/bollywood/todays-ent-wrap-tara-sutarias-apurva-gets-mixed-reviews-salman-khans-tiger-3-grosses-rs-240-crore-worldwide-and-more-article-105235345</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/videos/tv-serial-updates/bigg-boss-17-update-arun-mahashettys-shocking-comment-on-mannara-chopras-face-says-sadi-surat-video-105288286</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/sharer/sharer.php?u=https://www.zoomtventertainment.com/videos/tv-serial-updates/bigg-boss-17-update-arun-mahashettys-shocking-comment-on-mannara-chopras-face-says-sadi-surat-video-105288286</t>
+  </si>
+  <si>
+    <t>https://twitter.com/intent/tweet?text=Bigg%20Boss%2017%20update%20Arun%20Mahashettys%20SHOCKING%20comment%20on%20Mannara%20Chopras%20face%20says%20sadi%20surat&amp;url=https://www.zoomtventertainment.com/videos/tv-serial-updates/bigg-boss-17-update-arun-mahashettys-shocking-comment-on-mannara-chopras-face-says-sadi-surat-video-105288286</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/sharing/share-offsite/?url=https://www.zoomtventertainment.com/videos/tv-serial-updates/bigg-boss-17-update-arun-mahashettys-shocking-comment-on-mannara-chopras-face-says-sadi-surat-video-105288286</t>
+  </si>
+  <si>
+    <t>https://wa.me/?text=https://www.zoomtventertainment.com/videos/tv-serial-updates/bigg-boss-17-update-arun-mahashettys-shocking-comment-on-mannara-chopras-face-says-sadi-surat-video-105288286</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/videos/tv-serial-updates/bigg-boss-17-update-abhishek-kumar-insults-khanzaadi-during-diwali-celebrations-says-dil-todne-video-105285512</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/videos/tv-serial-updates/bigg-boss-17-new-promo-salman-khan-ne-uthaye-isha-malviya-ke-game-plan-par-savaal-isha-ke-ude-hosh-video-105284108</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/videos/bollywood-news-gossips/sumbul-touqeer-khans-20th-birthday-bash-on-the-set-of-kavya-ghkkpm-twist-savis-bold-move-slaps-samrudh-video-105269126</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/hollywood/will-pedro-pascal-play-reed-richards-in-marvels-fantastic-four-article-105266608</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/hollywood/madame-web-trailer-dakota-johnson-and-5-spider-man-characters-to-join-sonys-marvel-universe-article-105266598</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/hollywood/david-schwimmer-bids-farewell-to-friends-co-star-matthew-perry-thank-you-for-ten-incredible-years-of-laughter-article-105241948</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/hollywood/after-matt-leblanc-friends-star-courteney-cox-shares-emotional-post-remembering-matthew-perry-article-105226273</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/hollywood/matt-leblanc-pens-emotional-post-for-late-friend-matthew-perry-spread-your-wings-and-fly-brother-article-105216172</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/hollywood/anne-hathaway-was-told-her-career-would-fall-off-cliff-after-turning-35-actress-reveals-article-105214217</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/celebrity/david-beckham-attends-private-party-hosted-by-shah-rukh-khan-at-mannat-bollywood-news-entertainment-news-article-105278092</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/celebrity/somy-ali-says-salman-khan-has-a-knack-of-changing-girlfriends-claims-he-has-mental-issues-bollywood-news-entertainment-news-article-105265899</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/celebrity/fan-says-he-feel-insulted-after-nana-patekar-slapped-him-in-viral-video-bollywood-news-entertainment-news-article-105267105</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/celebrity/deepika-padukone-finally-reacts-to-open-relationship-controversy-im-okay-to-be-the-only-person-who-bollywood-news-entertainment-news-article-105266229</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/tamil-cinema/jigarthanda-doublex-box-office-collection-day-5-raghava-lawrence-film-hits-rs-25-crore-mark-article-105226382</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/tamil-cinema/jawan-director-atlee-responds-to-allegations-of-plagiarism-article-105222907</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/tamil-cinema/raja-magal-movie-review-aadukalam-murugadoss-film-gives-pivotal-lesson-on-excessive-parental-pampering-imdb-rating-public-review-review-105212771</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/tamil-cinema/jigarthanda-doublex-box-office-collection-day-4-karthik-subbarajs-film-surges-on-monday-article-105200530</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/telugu-cinema/telugu-star-rekha-boj-gets-trolled-for-her-wish-to-run-naked-on-vizag-beach-if-india-lifts-world-cup-trophy-entertainment-news-article-105264780</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/telugu-cinema/telugu-actor-vishwak-sen-rushed-to-hospital-after-he-fell-from-a-lorry-article-105242228</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/telugu-cinema/lavanya-tripathi-treats-fans-to-pics-with-hubby-varun-tej-from-their-first-diwali-post-wedding-fans-say-cute-couple-article-105207678</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/telugu-cinema/prabhas-salaar-part-1-ceasefire-trailer-set-to-release-on-this-date-article-105162695</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/malayalam-cinema/kaathal-the-core-trailer-mammootty-jyothika-promise-intriguing-political-drama-in-first-glimpse-watch-entertainment-news-malayalam-news-article-105203385</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/malayalam-cinema/prithviraj-sukumaran-unveils-l2-empuraans-first-poster-featuring-mohanlal-article-105154101</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/malayalam-cinema/malayalam-tv-actress-dr-priya-who-was-8-months-pregnant-dies-of-heart-attack-entertainment-news-article-104892497</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/malayalam-cinema/malayalam-star-renjusha-menon-35-found-dead-at-her-residence-entertainment-news-article-104826241</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/malayalam-cinema/director-alphonse-puthren-known-for-premam-quits-cinema-theatre-career-entertainment-news-malayalam-news-article-104825696</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/entertainment/animal-know-cast-salary-and-more-/photostory/105280449.cms</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/celebrity/just-9-cute-photos-of-aditya-roy-kapur-ananya-panday/photostory/105262090.cms</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/celebrity/aditya-roy-kapurs-iconic-performances-that-made-an-impact-aashiqui-2-yjhd-and-more/photostory/105259998.cms</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/8-delicious-desserts-to-try-this-festive-season-article-105073805</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/beauty/9-kitchen-ingredients-that-are-better-than-cosmetics-article-104801154</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/health-fitness/effective-ways-to-boost-metabolism-in-40s-article-104559385</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/grooming/hairstyling-advice-for-men-to-achieve-a-youthful-look-article-104502248</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/beauty/avoid-these-common-hair-oiling-mistakes-for-gorgeous-locks-article-104473555</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/health-fitness/nutritious-foods-you-can-eat-during-navratri-fasting-article-104445456</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/health-fitness/8-signs-of-insufficient-magnesium-levels-article-104443137</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/health-fitness/navratri-2023-8-fast-friendly-drinks-to-keep-you-hydrated-article-104375275</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/indian-cities-renowned-for-their-non-veg-delicacies-article-104365542</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/health/tips-to-get-rid-of-bed-bugs/photostory/104369906.cms</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/lifestyle/ways-to-build-strong-connection-with-your-baby-during-pregnancy/photostory/104368462.cms</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/make-5-different-chaat-recipes-in-the-comfort-of-your-home-article-104192055</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/travel/top-9-iconic-places-to-eat-desserts-in-india/photostory/103949961.cms</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/lifestyle/zodiac-signs-as-best-cooks/photostory/104108618.cms</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/lifestyle/consider-these-8-questions-to-ask-yourself-before-ending-a-relationship/photostory/103952206.cms</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/lifestyle/10-powerful-quotes-by-rumi/photostory/103965940.cms</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/lifestyle/indian-dishes-to-make-instantly-for-dinner-article-103607458</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/web-stories/health/fruits-and-vegetables-that-can-control-blood-sugar-levels/photostory/103598795.cms</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/zoomtv</t>
+  </si>
+  <si>
+    <t>https://twitter.com/ZoomTv</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/zoomtv</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/info/about-us</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/info/contact-us</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/info/advertise-with-us</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/info/regulatory-notices</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/info/terms-conditions</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/info/privacy-policy</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/info/disclaimer</t>
+  </si>
+  <si>
+    <t>https://www.zoomtventertainment.com/info/complaint-redressal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -320,6 +769,10 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -338,8 +791,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -361,8 +815,9 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{C00F39E2-DF54-4754-8049-3E89E8F52FC2}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -676,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1927,4 +2382,2334 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28586B4-5AA0-49C7-B13D-A817399D5150}">
+  <dimension ref="A1:C210"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="6">
+        <v>38</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="6">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="6">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A42" s="6">
+        <v>41</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A43" s="6">
+        <v>42</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A44" s="6">
+        <v>43</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A45" s="6">
+        <v>44</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A46" s="6">
+        <v>45</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
+        <v>46</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A48" s="6">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A49" s="6">
+        <v>48</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A50" s="6">
+        <v>49</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A51" s="6">
+        <v>50</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A52" s="6">
+        <v>51</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C52" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A53" s="6">
+        <v>52</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A54" s="6">
+        <v>53</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A55" s="6">
+        <v>54</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A56" s="6">
+        <v>55</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A57" s="6">
+        <v>56</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A58" s="6">
+        <v>57</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C58" s="6">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A59" s="6">
+        <v>58</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C59" s="6">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A60" s="6">
+        <v>59</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C60" s="6">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A61" s="6">
+        <v>60</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C61" s="6">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A62" s="6">
+        <v>61</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C62" s="6">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A63" s="6">
+        <v>62</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C63" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A64" s="6">
+        <v>63</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C64" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A65" s="6">
+        <v>64</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C65" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A66" s="6">
+        <v>65</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C66" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A67" s="6">
+        <v>66</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C67" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A68" s="6">
+        <v>67</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C68" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A69" s="6">
+        <v>68</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C69" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A70" s="6">
+        <v>69</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C70" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A71" s="6">
+        <v>70</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C71" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A72" s="6">
+        <v>71</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C72" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A73" s="6">
+        <v>72</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C73" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A74" s="6">
+        <v>73</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A75" s="6">
+        <v>74</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C75" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A76" s="6">
+        <v>75</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C76" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A77" s="6">
+        <v>76</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C77" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A78" s="6">
+        <v>77</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C78" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A79" s="6">
+        <v>78</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C79" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A80" s="6">
+        <v>79</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C80" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A81" s="6">
+        <v>80</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C81" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A82" s="6">
+        <v>81</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C82" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A83" s="6">
+        <v>82</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C83" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A84" s="6">
+        <v>83</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C84" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A85" s="6">
+        <v>84</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C85" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A86" s="6">
+        <v>85</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C86" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A87" s="6">
+        <v>86</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C87" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A88" s="6">
+        <v>87</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C88" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A89" s="6">
+        <v>88</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C89" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A90" s="6">
+        <v>89</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C90" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A91" s="6">
+        <v>90</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C91" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A92" s="6">
+        <v>91</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C92" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A93" s="6">
+        <v>92</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C93" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A94" s="6">
+        <v>93</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C94" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A95" s="6">
+        <v>94</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C95" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A96" s="6">
+        <v>95</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C96" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A97" s="6">
+        <v>96</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C97" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A98" s="6">
+        <v>97</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C98" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A99" s="6">
+        <v>98</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C99" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A100" s="6">
+        <v>99</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C100" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A101" s="6">
+        <v>100</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C101" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A102" s="6">
+        <v>101</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C102" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A103" s="6">
+        <v>102</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C103" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A104" s="6">
+        <v>103</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C104" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A105" s="6">
+        <v>104</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C105" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A106" s="6">
+        <v>105</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C106" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A107" s="6">
+        <v>106</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C107" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A108" s="6">
+        <v>107</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C108" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A109" s="6">
+        <v>108</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C109" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A110" s="6">
+        <v>109</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C110" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A111" s="6">
+        <v>110</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C111" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A112" s="6">
+        <v>111</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C112" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A113" s="6">
+        <v>112</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C113" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A114" s="6">
+        <v>113</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C114" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A115" s="6">
+        <v>114</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C115" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A116" s="6">
+        <v>115</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C116" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A117" s="6">
+        <v>116</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C117" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A118" s="6">
+        <v>117</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C118" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A119" s="6">
+        <v>118</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C119" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A120" s="6">
+        <v>119</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C120" s="6">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A121" s="6">
+        <v>120</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C121" s="6">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A122" s="6">
+        <v>121</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C122" s="6">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A123" s="6">
+        <v>122</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C123" s="6">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A124" s="6">
+        <v>123</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C124" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A125" s="6">
+        <v>124</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C125" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A126" s="6">
+        <v>125</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C126" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A127" s="6">
+        <v>126</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C127" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A128" s="6">
+        <v>127</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C128" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A129" s="6">
+        <v>128</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C129" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A130" s="6">
+        <v>129</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C130" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A131" s="6">
+        <v>130</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C131" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A132" s="6">
+        <v>131</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C132" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A133" s="6">
+        <v>132</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C133" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A134" s="6">
+        <v>133</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C134" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A135" s="6">
+        <v>134</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C135" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A136" s="6">
+        <v>135</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C136" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A137" s="6">
+        <v>136</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C137" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A138" s="6">
+        <v>137</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C138" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A139" s="6">
+        <v>138</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C139" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A140" s="6">
+        <v>139</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C140" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A141" s="6">
+        <v>140</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C141" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A142" s="6">
+        <v>141</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C142" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A143" s="6">
+        <v>142</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C143" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A144" s="6">
+        <v>143</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C144" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A145" s="6">
+        <v>144</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C145" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A146" s="6">
+        <v>145</v>
+      </c>
+      <c r="B146" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C146" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A147" s="6">
+        <v>146</v>
+      </c>
+      <c r="B147" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C147" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A148" s="6">
+        <v>147</v>
+      </c>
+      <c r="B148" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C148" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A149" s="6">
+        <v>148</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C149" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A150" s="6">
+        <v>149</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C150" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A151" s="6">
+        <v>150</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C151" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A152" s="6">
+        <v>151</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C152" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A153" s="6">
+        <v>152</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C153" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A154" s="6">
+        <v>153</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C154" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A155" s="6">
+        <v>154</v>
+      </c>
+      <c r="B155" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C155" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A156" s="6">
+        <v>155</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C156" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A157" s="6">
+        <v>156</v>
+      </c>
+      <c r="B157" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C157" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A158" s="6">
+        <v>157</v>
+      </c>
+      <c r="B158" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C158" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A159" s="6">
+        <v>158</v>
+      </c>
+      <c r="B159" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C159" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A160" s="6">
+        <v>159</v>
+      </c>
+      <c r="B160" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C160" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A161" s="6">
+        <v>160</v>
+      </c>
+      <c r="B161" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C161" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A162" s="6">
+        <v>161</v>
+      </c>
+      <c r="B162" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C162" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A163" s="6">
+        <v>162</v>
+      </c>
+      <c r="B163" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C163" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A164" s="6">
+        <v>163</v>
+      </c>
+      <c r="B164" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C164" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A165" s="6">
+        <v>164</v>
+      </c>
+      <c r="B165" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C165" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A166" s="6">
+        <v>165</v>
+      </c>
+      <c r="B166" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C166" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A167" s="6">
+        <v>166</v>
+      </c>
+      <c r="B167" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C167" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A168" s="6">
+        <v>167</v>
+      </c>
+      <c r="B168" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C168" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A169" s="6">
+        <v>168</v>
+      </c>
+      <c r="B169" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C169" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A170" s="6">
+        <v>169</v>
+      </c>
+      <c r="B170" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C170" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A171" s="6">
+        <v>170</v>
+      </c>
+      <c r="B171" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C171" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A172" s="6">
+        <v>171</v>
+      </c>
+      <c r="B172" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C172" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A173" s="6">
+        <v>172</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C173" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A174" s="6">
+        <v>173</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C174" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A175" s="6">
+        <v>174</v>
+      </c>
+      <c r="B175" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C175" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A176" s="6">
+        <v>175</v>
+      </c>
+      <c r="B176" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C176" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A177" s="6">
+        <v>176</v>
+      </c>
+      <c r="B177" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C177" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A178" s="6">
+        <v>177</v>
+      </c>
+      <c r="B178" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C178" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A179" s="6">
+        <v>178</v>
+      </c>
+      <c r="B179" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C179" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A180" s="6">
+        <v>179</v>
+      </c>
+      <c r="B180" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C180" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A181" s="6">
+        <v>180</v>
+      </c>
+      <c r="B181" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C181" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A182" s="6">
+        <v>181</v>
+      </c>
+      <c r="B182" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C182" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A183" s="6">
+        <v>182</v>
+      </c>
+      <c r="B183" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C183" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A184" s="6">
+        <v>183</v>
+      </c>
+      <c r="B184" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C184" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A185" s="6">
+        <v>184</v>
+      </c>
+      <c r="B185" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C185" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A186" s="6">
+        <v>185</v>
+      </c>
+      <c r="B186" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C186" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A187" s="6">
+        <v>186</v>
+      </c>
+      <c r="B187" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C187" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A188" s="6">
+        <v>187</v>
+      </c>
+      <c r="B188" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C188" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A189" s="6">
+        <v>188</v>
+      </c>
+      <c r="B189" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C189" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A190" s="6">
+        <v>189</v>
+      </c>
+      <c r="B190" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C190" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A191" s="6">
+        <v>190</v>
+      </c>
+      <c r="B191" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C191" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A192" s="6">
+        <v>191</v>
+      </c>
+      <c r="B192" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C192" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A193" s="6">
+        <v>192</v>
+      </c>
+      <c r="B193" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C193" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A194" s="6">
+        <v>193</v>
+      </c>
+      <c r="B194" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C194" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A195" s="6">
+        <v>194</v>
+      </c>
+      <c r="B195" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C195" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A196" s="6">
+        <v>195</v>
+      </c>
+      <c r="B196" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C196" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A197" s="6">
+        <v>196</v>
+      </c>
+      <c r="B197" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C197" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A198" s="6">
+        <v>197</v>
+      </c>
+      <c r="B198" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C198" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A199" s="6">
+        <v>198</v>
+      </c>
+      <c r="B199" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C199" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A200" s="6">
+        <v>199</v>
+      </c>
+      <c r="B200" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="C200" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A201" s="6">
+        <v>200</v>
+      </c>
+      <c r="B201" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C201" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A202" s="6">
+        <v>201</v>
+      </c>
+      <c r="B202" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C202" s="6">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A203" s="6">
+        <v>202</v>
+      </c>
+      <c r="B203" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C203" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A204" s="6">
+        <v>203</v>
+      </c>
+      <c r="B204" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C204" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A205" s="6">
+        <v>204</v>
+      </c>
+      <c r="B205" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C205" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A206" s="6">
+        <v>205</v>
+      </c>
+      <c r="B206" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C206" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A207" s="6">
+        <v>206</v>
+      </c>
+      <c r="B207" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C207" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A208" s="6">
+        <v>207</v>
+      </c>
+      <c r="B208" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C208" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A209" s="6">
+        <v>208</v>
+      </c>
+      <c r="B209" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C209" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A210" s="6">
+        <v>209</v>
+      </c>
+      <c r="B210" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C210" s="6">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>